<commit_message>
app6 dropMenu new dev
</commit_message>
<xml_diff>
--- a/data3.xlsx
+++ b/data3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>profile</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Scott</t>
+  </si>
+  <si>
+    <t>gruedisueli</t>
+  </si>
+  <si>
+    <t>Gavin</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1310,7 @@
         <v>0.2</v>
       </c>
       <c r="G2" s="3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H2" s="3">
         <v>1</v>
@@ -1425,17 +1431,39 @@
       </c>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="A6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.39</v>
+      </c>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="4"/>

</xml_diff>